<commit_message>
Add writeup for excel solution
</commit_message>
<xml_diff>
--- a/day 7 2021/Day 7.xlsx
+++ b/day 7 2021/Day 7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chee Hong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d82e34fa1d6b475/advent of code 2020/day 7 2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E30B67-26F2-4969-A574-295BE9500AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="13_ncr:1_{04E30B67-26F2-4969-A574-295BE9500AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C59D7321-45CA-49DF-8196-B682817D249C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-10368" windowWidth="13176" windowHeight="22656" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1" sheetId="3" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>location</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Set Objective to cell E3</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -9517,12 +9520,12 @@
   <dimension ref="A1:H1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="7" max="7" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
@@ -9552,7 +9555,7 @@
         <v>1101</v>
       </c>
       <c r="B2">
-        <f>ABS(A2-$E$1)*(ABS(A2-$E$1)+1)/2</f>
+        <f>((A2-$E$1)^2 + ABS(A2-$E$1))/2</f>
         <v>201930</v>
       </c>
       <c r="G2" t="s">
@@ -9567,7 +9570,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>ABS(A3-$E$1)*(ABS(A3-$E$1)+1)/2</f>
+        <f t="shared" ref="B3:B66" si="0">((A3-$E$1)^2 + ABS(A3-$E$1))/2</f>
         <v>108345</v>
       </c>
       <c r="D3" t="s">
@@ -9583,7 +9586,7 @@
         <v>29</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B67" si="0">ABS(A4-$E$1)*(ABS(A4-$E$1)+1)/2</f>
+        <f t="shared" si="0"/>
         <v>95703</v>
       </c>
     </row>
@@ -9616,6 +9619,13 @@
         <f t="shared" si="0"/>
         <v>108811</v>
       </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <f>AVERAGE(A2:A1001)</f>
+        <v>466.50400000000002</v>
+      </c>
       <c r="G7" t="s">
         <v>10</v>
       </c>
@@ -10156,7 +10166,7 @@
         <v>11</v>
       </c>
       <c r="B67">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B67:B130" si="1">((A67-$E$1)^2 + ABS(A67-$E$1))/2</f>
         <v>103740</v>
       </c>
     </row>
@@ -10165,7 +10175,7 @@
         <v>39</v>
       </c>
       <c r="B68">
-        <f t="shared" ref="B68:B131" si="1">ABS(A68-$E$1)*(ABS(A68-$E$1)+1)/2</f>
+        <f t="shared" si="1"/>
         <v>91378</v>
       </c>
     </row>
@@ -10732,7 +10742,7 @@
         <v>161</v>
       </c>
       <c r="B131">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B131:B194" si="2">((A131-$E$1)^2 + ABS(A131-$E$1))/2</f>
         <v>46665</v>
       </c>
     </row>
@@ -10741,7 +10751,7 @@
         <v>102</v>
       </c>
       <c r="B132">
-        <f t="shared" ref="B132:B195" si="2">ABS(A132-$E$1)*(ABS(A132-$E$1)+1)/2</f>
+        <f t="shared" si="2"/>
         <v>66430</v>
       </c>
     </row>
@@ -11308,7 +11318,7 @@
         <v>80</v>
       </c>
       <c r="B195">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="B195:B258" si="3">((A195-$E$1)^2 + ABS(A195-$E$1))/2</f>
         <v>74691</v>
       </c>
     </row>
@@ -11317,7 +11327,7 @@
         <v>540</v>
       </c>
       <c r="B196">
-        <f t="shared" ref="B196:B259" si="3">ABS(A196-$E$1)*(ABS(A196-$E$1)+1)/2</f>
+        <f t="shared" si="3"/>
         <v>2775</v>
       </c>
     </row>
@@ -11884,7 +11894,7 @@
         <v>685</v>
       </c>
       <c r="B259">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="B259:B322" si="4">((A259-$E$1)^2 + ABS(A259-$E$1))/2</f>
         <v>24090</v>
       </c>
     </row>
@@ -11893,7 +11903,7 @@
         <v>1083</v>
       </c>
       <c r="B260">
-        <f t="shared" ref="B260:B323" si="4">ABS(A260-$E$1)*(ABS(A260-$E$1)+1)/2</f>
+        <f t="shared" si="4"/>
         <v>190653</v>
       </c>
     </row>
@@ -12460,7 +12470,7 @@
         <v>262</v>
       </c>
       <c r="B323">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B323:B386" si="5">((A323-$E$1)^2 + ABS(A323-$E$1))/2</f>
         <v>20910</v>
       </c>
     </row>
@@ -12469,7 +12479,7 @@
         <v>87</v>
       </c>
       <c r="B324">
-        <f t="shared" ref="B324:B387" si="5">ABS(A324-$E$1)*(ABS(A324-$E$1)+1)/2</f>
+        <f t="shared" si="5"/>
         <v>72010</v>
       </c>
     </row>
@@ -13036,7 +13046,7 @@
         <v>1038</v>
       </c>
       <c r="B387">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="B387:B450" si="6">((A387-$E$1)^2 + ABS(A387-$E$1))/2</f>
         <v>163878</v>
       </c>
     </row>
@@ -13045,7 +13055,7 @@
         <v>688</v>
       </c>
       <c r="B388">
-        <f t="shared" ref="B388:B451" si="6">ABS(A388-$E$1)*(ABS(A388-$E$1)+1)/2</f>
+        <f t="shared" si="6"/>
         <v>24753</v>
       </c>
     </row>
@@ -13612,7 +13622,7 @@
         <v>462</v>
       </c>
       <c r="B451">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="B451:B514" si="7">((A451-$E$1)^2 + ABS(A451-$E$1))/2</f>
         <v>10</v>
       </c>
     </row>
@@ -13621,7 +13631,7 @@
         <v>260</v>
       </c>
       <c r="B452">
-        <f t="shared" ref="B452:B515" si="7">ABS(A452-$E$1)*(ABS(A452-$E$1)+1)/2</f>
+        <f t="shared" si="7"/>
         <v>21321</v>
       </c>
     </row>
@@ -14188,7 +14198,7 @@
         <v>238</v>
       </c>
       <c r="B515">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="B515:B578" si="8">((A515-$E$1)^2 + ABS(A515-$E$1))/2</f>
         <v>26106</v>
       </c>
     </row>
@@ -14197,7 +14207,7 @@
         <v>854</v>
       </c>
       <c r="B516">
-        <f t="shared" ref="B516:B579" si="8">ABS(A516-$E$1)*(ABS(A516-$E$1)+1)/2</f>
+        <f t="shared" si="8"/>
         <v>75466</v>
       </c>
     </row>
@@ -14764,7 +14774,7 @@
         <v>863</v>
       </c>
       <c r="B579">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="B579:B642" si="9">((A579-$E$1)^2 + ABS(A579-$E$1))/2</f>
         <v>79003</v>
       </c>
     </row>
@@ -14773,7 +14783,7 @@
         <v>11</v>
       </c>
       <c r="B580">
-        <f t="shared" ref="B580:B643" si="9">ABS(A580-$E$1)*(ABS(A580-$E$1)+1)/2</f>
+        <f t="shared" si="9"/>
         <v>103740</v>
       </c>
     </row>
@@ -15340,7 +15350,7 @@
         <v>1364</v>
       </c>
       <c r="B643">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="B643:B706" si="10">((A643-$E$1)^2 + ABS(A643-$E$1))/2</f>
         <v>403651</v>
       </c>
     </row>
@@ -15349,7 +15359,7 @@
         <v>130</v>
       </c>
       <c r="B644">
-        <f t="shared" ref="B644:B707" si="10">ABS(A644-$E$1)*(ABS(A644-$E$1)+1)/2</f>
+        <f t="shared" si="10"/>
         <v>56616</v>
       </c>
     </row>
@@ -15916,7 +15926,7 @@
         <v>201</v>
       </c>
       <c r="B707">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="B707:B770" si="11">((A707-$E$1)^2 + ABS(A707-$E$1))/2</f>
         <v>35245</v>
       </c>
     </row>
@@ -15925,7 +15935,7 @@
         <v>184</v>
       </c>
       <c r="B708">
-        <f t="shared" ref="B708:B771" si="11">ABS(A708-$E$1)*(ABS(A708-$E$1)+1)/2</f>
+        <f t="shared" si="11"/>
         <v>39903</v>
       </c>
     </row>
@@ -16492,7 +16502,7 @@
         <v>44</v>
       </c>
       <c r="B771">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="B771:B834" si="12">((A771-$E$1)^2 + ABS(A771-$E$1))/2</f>
         <v>89253</v>
       </c>
     </row>
@@ -16501,7 +16511,7 @@
         <v>621</v>
       </c>
       <c r="B772">
-        <f t="shared" ref="B772:B835" si="12">ABS(A772-$E$1)*(ABS(A772-$E$1)+1)/2</f>
+        <f t="shared" si="12"/>
         <v>12090</v>
       </c>
     </row>
@@ -17068,7 +17078,7 @@
         <v>12</v>
       </c>
       <c r="B835">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="B835:B898" si="13">((A835-$E$1)^2 + ABS(A835-$E$1))/2</f>
         <v>103285</v>
       </c>
     </row>
@@ -17077,7 +17087,7 @@
         <v>924</v>
       </c>
       <c r="B836">
-        <f t="shared" ref="B836:B899" si="13">ABS(A836-$E$1)*(ABS(A836-$E$1)+1)/2</f>
+        <f t="shared" si="13"/>
         <v>105111</v>
       </c>
     </row>
@@ -17644,7 +17654,7 @@
         <v>467</v>
       </c>
       <c r="B899">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="B899:B962" si="14">((A899-$E$1)^2 + ABS(A899-$E$1))/2</f>
         <v>1</v>
       </c>
     </row>
@@ -17653,7 +17663,7 @@
         <v>1848</v>
       </c>
       <c r="B900">
-        <f t="shared" ref="B900:B963" si="14">ABS(A900-$E$1)*(ABS(A900-$E$1)+1)/2</f>
+        <f t="shared" si="14"/>
         <v>955653</v>
       </c>
     </row>
@@ -18220,7 +18230,7 @@
         <v>1</v>
       </c>
       <c r="B963">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="B963:B1001" si="15">((A963-$E$1)^2 + ABS(A963-$E$1))/2</f>
         <v>108345</v>
       </c>
     </row>
@@ -18229,7 +18239,7 @@
         <v>229</v>
       </c>
       <c r="B964">
-        <f t="shared" ref="B964:B1001" si="15">ABS(A964-$E$1)*(ABS(A964-$E$1)+1)/2</f>
+        <f t="shared" si="15"/>
         <v>28203</v>
       </c>
     </row>

</xml_diff>